<commit_message>
Create 299 Scaled Data
</commit_message>
<xml_diff>
--- a/model/data/All_EVProject2013Qtly_Residential_Hr_AggDmd.xlsx
+++ b/model/data/All_EVProject2013Qtly_Residential_Hr_AggDmd.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF62E6-776F-41BF-A5E2-40EB1452D733}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -146,7 +147,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -424,25 +425,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG7" sqref="AG7"/>
+      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -538,7 +539,7 @@
         <v>8.6740389411240182E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -587,7 +588,7 @@
         <v>9.0631152366159665E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -636,7 +637,7 @@
         <v>7.2877539666058838E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>0.125</v>
       </c>
@@ -685,7 +686,7 @@
         <v>4.8635716685980573E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>0.16666666666666666</v>
       </c>
@@ -734,7 +735,7 @@
         <v>2.5792646903548624E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -783,7 +784,7 @@
         <v>1.1570736334075781E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>0.25</v>
       </c>
@@ -832,7 +833,7 @@
         <v>9.0193786940989291E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>0.29166666666666669</v>
       </c>
@@ -881,7 +882,7 @@
         <v>1.2744204417242815E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>0.33333333333333331</v>
       </c>
@@ -930,7 +931,7 @@
         <v>1.2855505136569821E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>0.375</v>
       </c>
@@ -979,7 +980,7 @@
         <v>1.2716439623295325E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>1.1254133778477393E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>0.45833333333333331</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>1.519397838013338E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>0.5</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>1.7691918666883015E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>0.54166666666666663</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>2.4578616032813621E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>0.58333333333333337</v>
       </c>
@@ -1224,7 +1225,7 @@
         <v>2.8914210650763165E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>0.625</v>
       </c>
@@ -1273,7 +1274,7 @@
         <v>3.0546170319623558E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>0.66666666666666663</v>
       </c>
@@ -1322,7 +1323,7 @@
         <v>3.1755489820103497E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>0.70833333333333337</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>4.04723663804019E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>0.75</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>5.8032278961702419E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>0.79166666666666663</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>6.6882556203689894E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>0.83333333333333337</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>7.4188276941353506E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>0.875</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>7.640548388776236E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>0.91666666666666663</v>
       </c>
@@ -1616,7 +1617,7 @@
         <v>7.3177979145180469E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>0.95833333333333337</v>
       </c>
@@ -1665,7 +1666,7 @@
         <v>6.7322831592841276E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>

</xml_diff>